<commit_message>
Commit Qualitative Progress 10
</commit_message>
<xml_diff>
--- a/Database_backup/Contract-2020-08-09.xlsx
+++ b/Database_backup/Contract-2020-08-09.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\website\cmis6\Database_backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Website_26_07_2020\cmis6\Database_backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17115" windowHeight="7440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17112" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="155">
   <si>
     <t>id</t>
   </si>
@@ -478,6 +478,15 @@
   </si>
   <si>
     <t>2016-12-13</t>
+  </si>
+  <si>
+    <t>NETR/PW-08</t>
+  </si>
+  <si>
+    <t>BWDB/ Netr/HFMLIP/PW-08 Dampara &amp; Singer Beel (Re-hab. Haor)</t>
+  </si>
+  <si>
+    <t>GS-SI (JV)</t>
   </si>
 </sst>
 </file>
@@ -825,19 +834,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18:U18"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="64.21875" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -902,7 +913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>49</v>
       </c>
@@ -925,7 +936,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>48</v>
       </c>
@@ -948,7 +959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>47</v>
       </c>
@@ -971,7 +982,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>41</v>
       </c>
@@ -997,7 +1008,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1023,7 +1034,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>39</v>
       </c>
@@ -1049,7 +1060,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>38</v>
       </c>
@@ -1075,7 +1086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>37</v>
       </c>
@@ -1101,7 +1112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>36</v>
       </c>
@@ -1124,7 +1135,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>35</v>
       </c>
@@ -1147,7 +1158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>34</v>
       </c>
@@ -1170,7 +1181,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>33</v>
       </c>
@@ -1196,7 +1207,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>32</v>
       </c>
@@ -1222,7 +1233,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>31</v>
       </c>
@@ -1245,7 +1256,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>30</v>
       </c>
@@ -1268,7 +1279,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>29</v>
       </c>
@@ -1291,7 +1302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>28</v>
       </c>
@@ -1317,7 +1328,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>27</v>
       </c>
@@ -1343,7 +1354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>26</v>
       </c>
@@ -1369,7 +1380,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>25</v>
       </c>
@@ -1395,7 +1406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>24</v>
       </c>
@@ -1421,7 +1432,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1447,7 +1458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1473,7 +1484,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1499,7 +1510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>20</v>
       </c>
@@ -1525,7 +1536,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>19</v>
       </c>
@@ -1551,7 +1562,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>18</v>
       </c>
@@ -1577,7 +1588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>17</v>
       </c>
@@ -1603,7 +1614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>16</v>
       </c>
@@ -1629,7 +1640,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1655,7 +1666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>14</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>13</v>
       </c>
@@ -1707,7 +1718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>12</v>
       </c>
@@ -1733,7 +1744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>11</v>
       </c>
@@ -1759,7 +1770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10</v>
       </c>
@@ -1785,7 +1796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>9</v>
       </c>
@@ -1811,7 +1822,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -1837,7 +1848,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7</v>
       </c>
@@ -1863,7 +1874,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>6</v>
       </c>
@@ -1889,7 +1900,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>5</v>
       </c>
@@ -1915,7 +1926,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1941,7 +1952,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>3</v>
       </c>
@@ -1967,7 +1978,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1993,7 +2004,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
@@ -2017,6 +2028,29 @@
       </c>
       <c r="J45" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="I46" t="s">
+        <v>24</v>
+      </c>
+      <c r="J46" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>